<commit_message>
scraped some more data
</commit_message>
<xml_diff>
--- a/cake_data.xlsx
+++ b/cake_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cake_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Git\cake_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -67,11 +67,23 @@
   <si>
     <t>Release</t>
   </si>
+  <si>
+    <t>Pastries</t>
+  </si>
+  <si>
+    <t>Treats</t>
+  </si>
+  <si>
+    <t>Pie</t>
+  </si>
+  <si>
+    <t>Cheesecake</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -201,23 +213,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -253,23 +248,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +531,7 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -609,7 +587,7 @@
         <v>0.51736111111111105</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -721,7 +699,7 @@
         <v>0.57222222222222219</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -973,7 +951,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -987,7 +965,7 @@
         <v>0.34513888888888888</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -1183,7 +1161,7 @@
         <v>0.55069444444444449</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -1230,6 +1208,820 @@
       <c r="D57" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>42489</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>42487</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>42487</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>42486</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>42481</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.51944444444444449</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>42480</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>42480</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>42478</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>42473</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>42468</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>42468</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.58472222222222225</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>42465</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.61875000000000002</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>42458</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>42458</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>42458</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.45277777777777778</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>42452</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="C73" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>42452</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="C74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>42450</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="C75" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>42446</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.61388888888888882</v>
+      </c>
+      <c r="C76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>42446</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="C77" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>42443</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.55486111111111114</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>42437</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.56736111111111109</v>
+      </c>
+      <c r="C79" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>42437</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="C80" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>42436</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>42432</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C82" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>42431</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="C83" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>42431</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>42426</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="C85" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>42425</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.62638888888888888</v>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>42422</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>42419</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="C88" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>42419</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>42419</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="C90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>42419</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>42411</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>42410</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="C93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>42405</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.62083333333333335</v>
+      </c>
+      <c r="C94" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>42404</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>42402</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.4694444444444445</v>
+      </c>
+      <c r="C96" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>42398</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>42398</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.57013888888888886</v>
+      </c>
+      <c r="C98" t="s">
+        <v>3</v>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>42396</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.68263888888888891</v>
+      </c>
+      <c r="C99" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>42391</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>42390</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="C101" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>42390</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="C102" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>42390</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C103" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>42389</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="C104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>42388</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="C105" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>42387</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0.6020833333333333</v>
+      </c>
+      <c r="C106" t="s">
+        <v>3</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>42383</v>
+      </c>
+      <c r="B107" s="2">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="C107" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>42382</v>
+      </c>
+      <c r="B108" s="2">
+        <v>0.40763888888888888</v>
+      </c>
+      <c r="C108" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>42376</v>
+      </c>
+      <c r="B109" s="2">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>42375</v>
+      </c>
+      <c r="B110" s="2">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="C110" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
there were doughnuts today
</commit_message>
<xml_diff>
--- a/cake_data.xlsx
+++ b/cake_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -117,10 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,13 +429,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42593</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.42499999999999999</v>
+        <v>42594</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.52083333333333337</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -442,13 +443,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42590</v>
+        <v>42593</v>
       </c>
       <c r="B3" s="2">
-        <v>0.65416666666666667</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -459,7 +460,7 @@
         <v>42590</v>
       </c>
       <c r="B4" s="2">
-        <v>0.55972222222222223</v>
+        <v>0.65416666666666667</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -470,13 +471,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>42587</v>
+        <v>42590</v>
       </c>
       <c r="B5" s="2">
-        <v>0.54999999999999993</v>
+        <v>0.55972222222222223</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -484,13 +485,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>42583</v>
+        <v>42587</v>
       </c>
       <c r="B6" s="2">
-        <v>0.52638888888888891</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -501,10 +502,10 @@
         <v>42583</v>
       </c>
       <c r="B7" s="2">
-        <v>0.52430555555555558</v>
+        <v>0.52638888888888891</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -515,10 +516,10 @@
         <v>42583</v>
       </c>
       <c r="B8" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -529,10 +530,10 @@
         <v>42583</v>
       </c>
       <c r="B9" s="2">
-        <v>0.41388888888888892</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -540,13 +541,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>42580</v>
+        <v>42583</v>
       </c>
       <c r="B10" s="2">
-        <v>0.53333333333333333</v>
+        <v>0.41388888888888892</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -554,13 +555,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>42579</v>
+        <v>42580</v>
       </c>
       <c r="B11" s="2">
-        <v>0.5708333333333333</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -568,13 +569,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>42573</v>
+        <v>42579</v>
       </c>
       <c r="B12" s="2">
-        <v>0.63888888888888895</v>
+        <v>0.5708333333333333</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -582,13 +583,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>42572</v>
+        <v>42573</v>
       </c>
       <c r="B13" s="2">
-        <v>0.54236111111111118</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -596,13 +597,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>42571</v>
+        <v>42572</v>
       </c>
       <c r="B14" s="2">
-        <v>0.51736111111111105</v>
+        <v>0.54236111111111118</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -610,13 +611,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>42570</v>
+        <v>42571</v>
       </c>
       <c r="B15" s="2">
-        <v>0.58819444444444446</v>
+        <v>0.51736111111111105</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -624,13 +625,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>42569</v>
+        <v>42570</v>
       </c>
       <c r="B16" s="2">
-        <v>0.61458333333333337</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -641,10 +642,10 @@
         <v>42569</v>
       </c>
       <c r="B17" s="2">
-        <v>0.4152777777777778</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -652,16 +653,16 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>42566</v>
+        <v>42569</v>
       </c>
       <c r="B18" s="2">
-        <v>0.61875000000000002</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -669,24 +670,24 @@
         <v>42566</v>
       </c>
       <c r="B19" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.61875000000000002</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>42565</v>
+        <v>42566</v>
       </c>
       <c r="B20" s="2">
-        <v>0.45277777777777778</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -694,13 +695,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>42563</v>
+        <v>42565</v>
       </c>
       <c r="B21" s="2">
-        <v>0.34375</v>
+        <v>0.45277777777777778</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -708,13 +709,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>42559</v>
+        <v>42563</v>
       </c>
       <c r="B22" s="2">
-        <v>0.57222222222222219</v>
+        <v>0.34375</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -722,13 +723,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>42557</v>
+        <v>42559</v>
       </c>
       <c r="B23" s="2">
-        <v>0.3979166666666667</v>
+        <v>0.57222222222222219</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -736,13 +737,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>42556</v>
+        <v>42557</v>
       </c>
       <c r="B24" s="2">
-        <v>0.37083333333333335</v>
+        <v>0.3979166666666667</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -750,13 +751,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>42555</v>
+        <v>42556</v>
       </c>
       <c r="B25" s="2">
-        <v>0.40902777777777777</v>
+        <v>0.37083333333333335</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -764,13 +765,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>42551</v>
+        <v>42555</v>
       </c>
       <c r="B26" s="2">
-        <v>0.41319444444444442</v>
+        <v>0.40902777777777777</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -778,13 +779,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>42549</v>
+        <v>42551</v>
       </c>
       <c r="B27" s="2">
-        <v>0.38055555555555554</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -792,13 +793,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>42545</v>
+        <v>42549</v>
       </c>
       <c r="B28" s="2">
-        <v>0.56597222222222221</v>
+        <v>0.38055555555555554</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -809,10 +810,10 @@
         <v>42545</v>
       </c>
       <c r="B29" s="2">
-        <v>0.55625000000000002</v>
+        <v>0.56597222222222221</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -823,10 +824,10 @@
         <v>42545</v>
       </c>
       <c r="B30" s="2">
-        <v>0.47430555555555554</v>
+        <v>0.55625000000000002</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -834,13 +835,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>42544</v>
+        <v>42545</v>
       </c>
       <c r="B31" s="2">
-        <v>0.62708333333333333</v>
+        <v>0.47430555555555554</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -851,7 +852,7 @@
         <v>42544</v>
       </c>
       <c r="B32" s="2">
-        <v>0.55347222222222225</v>
+        <v>0.62708333333333333</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -862,13 +863,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>42541</v>
+        <v>42544</v>
       </c>
       <c r="B33" s="2">
-        <v>0.51250000000000007</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -876,10 +877,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>42538</v>
+        <v>42541</v>
       </c>
       <c r="B34" s="2">
-        <v>0.67569444444444438</v>
+        <v>0.51250000000000007</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -890,13 +891,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>42537</v>
+        <v>42538</v>
       </c>
       <c r="B35" s="2">
-        <v>0.46180555555555558</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -904,13 +905,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>42536</v>
+        <v>42537</v>
       </c>
       <c r="B36" s="2">
-        <v>0.60416666666666663</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -918,13 +919,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>42535</v>
+        <v>42536</v>
       </c>
       <c r="B37" s="2">
-        <v>0.35902777777777778</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -932,13 +933,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>42524</v>
+        <v>42535</v>
       </c>
       <c r="B38" s="2">
-        <v>0.58680555555555558</v>
+        <v>0.35902777777777778</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -946,13 +947,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>42523</v>
+        <v>42524</v>
       </c>
       <c r="B39" s="2">
-        <v>0.53333333333333333</v>
+        <v>0.58680555555555558</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -960,13 +961,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>42517</v>
+        <v>42523</v>
       </c>
       <c r="B40" s="2">
-        <v>0.57916666666666672</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -974,10 +975,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>42516</v>
+        <v>42517</v>
       </c>
       <c r="B41" s="2">
-        <v>0.34513888888888888</v>
+        <v>0.57916666666666672</v>
       </c>
       <c r="C41" t="s">
         <v>15</v>
@@ -988,13 +989,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>42514</v>
+        <v>42516</v>
       </c>
       <c r="B42" s="2">
-        <v>0.36805555555555558</v>
+        <v>0.34513888888888888</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -1002,13 +1003,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42513</v>
+        <v>42514</v>
       </c>
       <c r="B43" s="2">
-        <v>0.36041666666666666</v>
+        <v>0.36805555555555558</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -1016,10 +1017,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42510</v>
+        <v>42513</v>
       </c>
       <c r="B44" s="2">
-        <v>0.59930555555555554</v>
+        <v>0.36041666666666666</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
@@ -1030,13 +1031,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>42503</v>
+        <v>42510</v>
       </c>
       <c r="B45" s="2">
-        <v>0.70486111111111116</v>
+        <v>0.59930555555555554</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -1047,10 +1048,10 @@
         <v>42503</v>
       </c>
       <c r="B46" s="2">
-        <v>0.66736111111111107</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -1061,10 +1062,10 @@
         <v>42503</v>
       </c>
       <c r="B47" s="2">
-        <v>0.47500000000000003</v>
+        <v>0.66736111111111107</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -1075,7 +1076,7 @@
         <v>42503</v>
       </c>
       <c r="B48" s="2">
-        <v>0.37013888888888885</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
@@ -1089,7 +1090,7 @@
         <v>42503</v>
       </c>
       <c r="B49" s="2">
-        <v>0.5805555555555556</v>
+        <v>0.37013888888888885</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -1100,13 +1101,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>42502</v>
+        <v>42503</v>
       </c>
       <c r="B50" s="2">
-        <v>0.4597222222222222</v>
+        <v>0.5805555555555556</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -1117,10 +1118,10 @@
         <v>42502</v>
       </c>
       <c r="B51" s="2">
-        <v>0.39999999999999997</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -1128,27 +1129,27 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>42501</v>
+        <v>42502</v>
       </c>
       <c r="B52" s="2">
-        <v>0.48194444444444445</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>42500</v>
+        <v>42501</v>
       </c>
       <c r="B53" s="2">
-        <v>0.61527777777777781</v>
+        <v>0.48194444444444445</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -1159,13 +1160,13 @@
         <v>42500</v>
       </c>
       <c r="B54" s="2">
-        <v>0.57222222222222219</v>
+        <v>0.61527777777777781</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1173,10 +1174,10 @@
         <v>42500</v>
       </c>
       <c r="B55" s="2">
-        <v>0.55069444444444449</v>
+        <v>0.57222222222222219</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -1184,13 +1185,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>42499</v>
+        <v>42500</v>
       </c>
       <c r="B56" s="2">
-        <v>0.6479166666666667</v>
+        <v>0.55069444444444449</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -1198,10 +1199,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>42496</v>
+        <v>42499</v>
       </c>
       <c r="B57" s="2">
-        <v>0.58194444444444449</v>
+        <v>0.6479166666666667</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
@@ -1212,10 +1213,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>42492</v>
+        <v>42496</v>
       </c>
       <c r="B58" s="2">
-        <v>0.38541666666666669</v>
+        <v>0.58194444444444449</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
@@ -1226,13 +1227,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>42489</v>
+        <v>42492</v>
       </c>
       <c r="B59" s="2">
-        <v>0.54375000000000007</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -1240,16 +1241,16 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>42487</v>
+        <v>42489</v>
       </c>
       <c r="B60" s="2">
-        <v>0.57152777777777775</v>
+        <v>0.54375000000000007</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,7 +1258,7 @@
         <v>42487</v>
       </c>
       <c r="B61" s="2">
-        <v>0.4145833333333333</v>
+        <v>0.57152777777777775</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
@@ -1268,24 +1269,24 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>42486</v>
+        <v>42487</v>
       </c>
       <c r="B62" s="2">
-        <v>0.54999999999999993</v>
+        <v>0.4145833333333333</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
       </c>
       <c r="D62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>42481</v>
+        <v>42486</v>
       </c>
       <c r="B63" s="2">
-        <v>0.51944444444444449</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -1296,16 +1297,16 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>42480</v>
+        <v>42481</v>
       </c>
       <c r="B64" s="2">
-        <v>0.5493055555555556</v>
+        <v>0.51944444444444449</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
       </c>
       <c r="D64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1313,24 +1314,24 @@
         <v>42480</v>
       </c>
       <c r="B65" s="2">
-        <v>0.34930555555555554</v>
+        <v>0.5493055555555556</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>42478</v>
+        <v>42480</v>
       </c>
       <c r="B66" s="2">
-        <v>0.42083333333333334</v>
+        <v>0.34930555555555554</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -1338,13 +1339,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>42473</v>
+        <v>42478</v>
       </c>
       <c r="B67" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.42083333333333334</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -1352,16 +1353,16 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>42468</v>
+        <v>42473</v>
       </c>
       <c r="B68" s="2">
-        <v>0.60555555555555551</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C68" t="s">
         <v>3</v>
       </c>
       <c r="D68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1369,24 +1370,24 @@
         <v>42468</v>
       </c>
       <c r="B69" s="2">
-        <v>0.58472222222222225</v>
+        <v>0.60555555555555551</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
       </c>
       <c r="D69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>42465</v>
+        <v>42468</v>
       </c>
       <c r="B70" s="2">
-        <v>0.61875000000000002</v>
+        <v>0.58472222222222225</v>
       </c>
       <c r="C70" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -1394,13 +1395,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>42458</v>
+        <v>42465</v>
       </c>
       <c r="B71" s="2">
-        <v>0.6166666666666667</v>
+        <v>0.61875000000000002</v>
       </c>
       <c r="C71" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -1411,7 +1412,7 @@
         <v>42458</v>
       </c>
       <c r="B72" s="2">
-        <v>0.61527777777777781</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -1425,10 +1426,10 @@
         <v>42458</v>
       </c>
       <c r="B73" s="2">
-        <v>0.45277777777777778</v>
+        <v>0.61527777777777781</v>
       </c>
       <c r="C73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -1436,13 +1437,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>42452</v>
+        <v>42458</v>
       </c>
       <c r="B74" s="2">
-        <v>0.5625</v>
+        <v>0.45277777777777778</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -1453,10 +1454,10 @@
         <v>42452</v>
       </c>
       <c r="B75" s="2">
-        <v>0.45555555555555555</v>
+        <v>0.5625</v>
       </c>
       <c r="C75" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -1464,13 +1465,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>42450</v>
+        <v>42452</v>
       </c>
       <c r="B76" s="2">
-        <v>0.56597222222222221</v>
+        <v>0.45555555555555555</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -1478,13 +1479,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>42446</v>
+        <v>42450</v>
       </c>
       <c r="B77" s="2">
-        <v>0.61388888888888882</v>
+        <v>0.56597222222222221</v>
       </c>
       <c r="C77" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -1495,10 +1496,10 @@
         <v>42446</v>
       </c>
       <c r="B78" s="2">
-        <v>0.36041666666666666</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -1506,13 +1507,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>42443</v>
+        <v>42446</v>
       </c>
       <c r="B79" s="2">
-        <v>0.55486111111111114</v>
+        <v>0.36041666666666666</v>
       </c>
       <c r="C79" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -1520,13 +1521,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>42437</v>
+        <v>42443</v>
       </c>
       <c r="B80" s="2">
-        <v>0.56736111111111109</v>
+        <v>0.55486111111111114</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -1537,10 +1538,10 @@
         <v>42437</v>
       </c>
       <c r="B81" s="2">
-        <v>0.56597222222222221</v>
+        <v>0.56736111111111109</v>
       </c>
       <c r="C81" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -1548,13 +1549,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>42436</v>
+        <v>42437</v>
       </c>
       <c r="B82" s="2">
-        <v>0.62916666666666665</v>
+        <v>0.56597222222222221</v>
       </c>
       <c r="C82" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -1562,13 +1563,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>42432</v>
+        <v>42436</v>
       </c>
       <c r="B83" s="2">
-        <v>0.625</v>
+        <v>0.62916666666666665</v>
       </c>
       <c r="C83" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -1576,13 +1577,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>42431</v>
+        <v>42432</v>
       </c>
       <c r="B84" s="2">
-        <v>0.44861111111111113</v>
+        <v>0.625</v>
       </c>
       <c r="C84" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -1593,10 +1594,10 @@
         <v>42431</v>
       </c>
       <c r="B85" s="2">
-        <v>0.3527777777777778</v>
+        <v>0.44861111111111113</v>
       </c>
       <c r="C85" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -1604,10 +1605,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>42426</v>
+        <v>42431</v>
       </c>
       <c r="B86" s="2">
-        <v>0.43611111111111112</v>
+        <v>0.3527777777777778</v>
       </c>
       <c r="C86" t="s">
         <v>3</v>
@@ -1618,13 +1619,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>42425</v>
+        <v>42426</v>
       </c>
       <c r="B87" s="2">
-        <v>0.62638888888888888</v>
+        <v>0.43611111111111112</v>
       </c>
       <c r="C87" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -1632,13 +1633,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>42422</v>
+        <v>42425</v>
       </c>
       <c r="B88" s="2">
-        <v>0.47569444444444442</v>
+        <v>0.62638888888888888</v>
       </c>
       <c r="C88" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -1646,13 +1647,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>42419</v>
+        <v>42422</v>
       </c>
       <c r="B89" s="2">
-        <v>0.3576388888888889</v>
+        <v>0.47569444444444442</v>
       </c>
       <c r="C89" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -1663,10 +1664,10 @@
         <v>42419</v>
       </c>
       <c r="B90" s="2">
-        <v>0.5625</v>
+        <v>0.3576388888888889</v>
       </c>
       <c r="C90" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -1677,10 +1678,10 @@
         <v>42419</v>
       </c>
       <c r="B91" s="2">
-        <v>0.61319444444444449</v>
+        <v>0.5625</v>
       </c>
       <c r="C91" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -1691,94 +1692,94 @@
         <v>42419</v>
       </c>
       <c r="B92" s="2">
-        <v>0.6333333333333333</v>
+        <v>0.61319444444444449</v>
       </c>
       <c r="C92" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>42411</v>
+        <v>42419</v>
       </c>
       <c r="B93" s="2">
-        <v>0.41388888888888892</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="C93" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D93" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>42410</v>
+        <v>42411</v>
       </c>
       <c r="B94" s="2">
-        <v>0.6166666666666667</v>
+        <v>0.41388888888888892</v>
       </c>
       <c r="C94" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>42405</v>
+        <v>42410</v>
       </c>
       <c r="B95" s="2">
-        <v>0.62083333333333335</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
       </c>
       <c r="D95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>42404</v>
+        <v>42405</v>
       </c>
       <c r="B96" s="2">
-        <v>0.65486111111111112</v>
+        <v>0.62083333333333335</v>
       </c>
       <c r="C96" t="s">
         <v>3</v>
       </c>
       <c r="D96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>42402</v>
+        <v>42404</v>
       </c>
       <c r="B97" s="2">
-        <v>0.4694444444444445</v>
+        <v>0.65486111111111112</v>
       </c>
       <c r="C97" t="s">
         <v>3</v>
       </c>
       <c r="D97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>42398</v>
+        <v>42402</v>
       </c>
       <c r="B98" s="2">
-        <v>0.6118055555555556</v>
+        <v>0.4694444444444445</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -1789,35 +1790,35 @@
         <v>42398</v>
       </c>
       <c r="B99" s="2">
-        <v>0.57013888888888886</v>
+        <v>0.6118055555555556</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>42396</v>
+        <v>42398</v>
       </c>
       <c r="B100" s="2">
-        <v>0.68263888888888891</v>
+        <v>0.57013888888888886</v>
       </c>
       <c r="C100" t="s">
         <v>3</v>
       </c>
       <c r="D100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>42391</v>
+        <v>42396</v>
       </c>
       <c r="B101" s="2">
-        <v>0.63194444444444442</v>
+        <v>0.68263888888888891</v>
       </c>
       <c r="C101" t="s">
         <v>3</v>
@@ -1828,10 +1829,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>42390</v>
+        <v>42391</v>
       </c>
       <c r="B102" s="2">
-        <v>0.6743055555555556</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="C102" t="s">
         <v>3</v>
@@ -1845,7 +1846,7 @@
         <v>42390</v>
       </c>
       <c r="B103" s="2">
-        <v>0.63958333333333328</v>
+        <v>0.6743055555555556</v>
       </c>
       <c r="C103" t="s">
         <v>3</v>
@@ -1859,7 +1860,7 @@
         <v>42390</v>
       </c>
       <c r="B104" s="2">
-        <v>0.60416666666666663</v>
+        <v>0.63958333333333328</v>
       </c>
       <c r="C104" t="s">
         <v>3</v>
@@ -1870,10 +1871,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>42389</v>
+        <v>42390</v>
       </c>
       <c r="B105" s="2">
-        <v>0.4368055555555555</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C105" t="s">
         <v>3</v>
@@ -1884,10 +1885,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>42388</v>
+        <v>42389</v>
       </c>
       <c r="B106" s="2">
-        <v>0.60763888888888895</v>
+        <v>0.4368055555555555</v>
       </c>
       <c r="C106" t="s">
         <v>3</v>
@@ -1898,10 +1899,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>42387</v>
+        <v>42388</v>
       </c>
       <c r="B107" s="2">
-        <v>0.6020833333333333</v>
+        <v>0.60763888888888895</v>
       </c>
       <c r="C107" t="s">
         <v>3</v>
@@ -1912,41 +1913,41 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>42383</v>
+        <v>42387</v>
       </c>
       <c r="B108" s="2">
-        <v>0.57430555555555551</v>
+        <v>0.6020833333333333</v>
       </c>
       <c r="C108" t="s">
         <v>3</v>
       </c>
       <c r="D108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>42382</v>
+        <v>42383</v>
       </c>
       <c r="B109" s="2">
-        <v>0.40763888888888888</v>
+        <v>0.57430555555555551</v>
       </c>
       <c r="C109" t="s">
         <v>3</v>
       </c>
       <c r="D109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>42376</v>
+        <v>42382</v>
       </c>
       <c r="B110" s="2">
-        <v>0.37013888888888885</v>
+        <v>0.40763888888888888</v>
       </c>
       <c r="C110" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -1954,68 +1955,79 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
+        <v>42376</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C111" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
         <v>42375</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B112" s="2">
         <v>0.42222222222222222</v>
       </c>
-      <c r="C111" t="s">
-        <v>3</v>
-      </c>
-      <c r="D111" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="2"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
@@ -2038,6 +2050,9 @@
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>